<commit_message>
fix: incorrect test file
</commit_message>
<xml_diff>
--- a/test/tasker/importer/test-member-import-data.xlsx
+++ b/test/tasker/importer/test-member-import-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>test-member-import-data</t>
   </si>
@@ -31,6 +31,9 @@
     <t>星等</t>
   </si>
   <si>
+    <t>身份</t>
+  </si>
+  <si>
     <t>承辦人信箱</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t>建立日期</t>
   </si>
   <si>
+    <t>上次登入日期</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -82,6 +88,9 @@
     <t>star</t>
   </si>
   <si>
+    <t>role</t>
+  </si>
+  <si>
     <t>manager.email</t>
   </si>
   <si>
@@ -116,6 +125,9 @@
   </si>
   <si>
     <t>createdAt</t>
+  </si>
+  <si>
+    <t>loginedAt</t>
   </si>
   <si>
     <t>KK</t>
@@ -185,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -195,6 +207,11 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -209,7 +226,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +245,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -241,6 +264,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -257,13 +302,13 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -272,43 +317,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -317,26 +362,180 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -348,41 +547,89 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -402,8 +649,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -422,10 +671,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -602,11 +851,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -615,34 +867,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -890,12 +1142,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1186,7 +1438,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1467,7 +1719,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Q5"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1476,232 +1728,355 @@
     <col min="1" max="1" width="6.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.67188" style="1" customWidth="1"/>
     <col min="3" max="4" width="14.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6719" style="1" customWidth="1"/>
-    <col min="7" max="8" width="9.85156" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.35156" style="1" customWidth="1"/>
-    <col min="10" max="11" width="6" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3516" style="1" customWidth="1"/>
-    <col min="14" max="15" width="10.6719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.3516" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.67188" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="5" max="6" width="4.85156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6719" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.85156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.35156" style="1" customWidth="1"/>
+    <col min="11" max="12" width="6" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.3516" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.6719" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.3516" style="1" customWidth="1"/>
+    <col min="18" max="19" width="8.67188" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="N2" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="O2" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="P2" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="Q2" t="s" s="3">
+      <c r="Q2" t="s" s="7">
         <v>17</v>
+      </c>
+      <c r="R2" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="S2" t="s" s="7">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="6">
+      <c r="A3" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="B3" t="s" s="9">
         <v>21</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="C3" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="6">
+      <c r="D3" t="s" s="10">
         <v>23</v>
       </c>
-      <c r="G3" t="s" s="6">
+      <c r="E3" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="H3" t="s" s="6">
+      <c r="F3" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="G3" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="J3" t="s" s="6">
+      <c r="H3" t="s" s="10">
         <v>27</v>
       </c>
-      <c r="K3" t="s" s="6">
+      <c r="I3" t="s" s="10">
         <v>28</v>
       </c>
-      <c r="L3" t="s" s="6">
+      <c r="J3" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="M3" t="s" s="6">
+      <c r="K3" t="s" s="10">
         <v>30</v>
       </c>
-      <c r="N3" t="s" s="6">
+      <c r="L3" t="s" s="10">
         <v>31</v>
       </c>
-      <c r="O3" t="s" s="6">
+      <c r="M3" t="s" s="10">
         <v>32</v>
       </c>
-      <c r="P3" t="s" s="6">
+      <c r="N3" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="Q3" t="s" s="6">
+      <c r="O3" t="s" s="10">
         <v>34</v>
+      </c>
+      <c r="P3" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s" s="10">
+        <v>38</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="A4" s="11"/>
+      <c r="B4" t="s" s="12">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="E4" s="14">
         <v>999</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="14">
         <v>987654321</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="14">
         <v>900000000</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" t="s" s="9">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="O4" s="11"/>
-      <c r="P4" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="11"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" t="s" s="13">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="8">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s" s="12">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s" s="13">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s" s="13">
+        <v>46</v>
+      </c>
+      <c r="E5" s="14">
         <v>0</v>
       </c>
-      <c r="F5" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="F5" s="15"/>
+      <c r="G5" t="s" s="13">
+        <v>47</v>
+      </c>
+      <c r="H5" s="14">
         <v>912345678</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="K5" s="11"/>
-      <c r="L5" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="M5" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" t="s" s="13">
+        <v>48</v>
+      </c>
+      <c r="L5" s="15"/>
+      <c r="M5" t="s" s="13">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s" s="13">
+        <v>50</v>
+      </c>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="23"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="23"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="23"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="" tooltip="" display="kk@example.com"/>
     <hyperlink ref="D4" r:id="rId2" location="" tooltip="" display="kk@example.com"/>
     <hyperlink ref="C5" r:id="rId3" location="" tooltip="" display="zz@example.com"/>
     <hyperlink ref="D5" r:id="rId4" location="" tooltip="" display="zz@example.com"/>
-    <hyperlink ref="F5" r:id="rId5" location="" tooltip="" display="sales@example.com"/>
+    <hyperlink ref="G5" r:id="rId5" location="" tooltip="" display="sales@example.com"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Supplementary/missing filed at mebmer export (#26)
* test: cases for loginedAt & role fields

* fix: missing loginedAt & role fields

* fix: incorrect test file
</commit_message>
<xml_diff>
--- a/test/tasker/importer/test-member-import-data.xlsx
+++ b/test/tasker/importer/test-member-import-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>test-member-import-data</t>
   </si>
@@ -31,6 +31,9 @@
     <t>星等</t>
   </si>
   <si>
+    <t>身份</t>
+  </si>
+  <si>
     <t>承辦人信箱</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t>建立日期</t>
   </si>
   <si>
+    <t>上次登入日期</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -82,6 +88,9 @@
     <t>star</t>
   </si>
   <si>
+    <t>role</t>
+  </si>
+  <si>
     <t>manager.email</t>
   </si>
   <si>
@@ -116,6 +125,9 @@
   </si>
   <si>
     <t>createdAt</t>
+  </si>
+  <si>
+    <t>loginedAt</t>
   </si>
   <si>
     <t>KK</t>
@@ -185,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -195,6 +207,11 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -209,7 +226,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +245,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -241,6 +264,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -257,13 +302,13 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -272,43 +317,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -317,26 +362,180 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -348,41 +547,89 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -402,8 +649,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -422,10 +671,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -602,11 +851,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -615,34 +867,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -890,12 +1142,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1186,7 +1438,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1467,7 +1719,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Q5"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1476,232 +1728,355 @@
     <col min="1" max="1" width="6.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.67188" style="1" customWidth="1"/>
     <col min="3" max="4" width="14.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6719" style="1" customWidth="1"/>
-    <col min="7" max="8" width="9.85156" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.35156" style="1" customWidth="1"/>
-    <col min="10" max="11" width="6" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3516" style="1" customWidth="1"/>
-    <col min="14" max="15" width="10.6719" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.3516" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.67188" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="5" max="6" width="4.85156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6719" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.85156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.35156" style="1" customWidth="1"/>
+    <col min="11" max="12" width="6" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.3516" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.6719" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.3516" style="1" customWidth="1"/>
+    <col min="18" max="19" width="8.67188" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="N2" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="O2" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="P2" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="Q2" t="s" s="3">
+      <c r="Q2" t="s" s="7">
         <v>17</v>
+      </c>
+      <c r="R2" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="S2" t="s" s="7">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="6">
+      <c r="A3" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="B3" t="s" s="9">
         <v>21</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="C3" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="6">
+      <c r="D3" t="s" s="10">
         <v>23</v>
       </c>
-      <c r="G3" t="s" s="6">
+      <c r="E3" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="H3" t="s" s="6">
+      <c r="F3" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="G3" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="J3" t="s" s="6">
+      <c r="H3" t="s" s="10">
         <v>27</v>
       </c>
-      <c r="K3" t="s" s="6">
+      <c r="I3" t="s" s="10">
         <v>28</v>
       </c>
-      <c r="L3" t="s" s="6">
+      <c r="J3" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="M3" t="s" s="6">
+      <c r="K3" t="s" s="10">
         <v>30</v>
       </c>
-      <c r="N3" t="s" s="6">
+      <c r="L3" t="s" s="10">
         <v>31</v>
       </c>
-      <c r="O3" t="s" s="6">
+      <c r="M3" t="s" s="10">
         <v>32</v>
       </c>
-      <c r="P3" t="s" s="6">
+      <c r="N3" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="Q3" t="s" s="6">
+      <c r="O3" t="s" s="10">
         <v>34</v>
+      </c>
+      <c r="P3" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s" s="10">
+        <v>38</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="A4" s="11"/>
+      <c r="B4" t="s" s="12">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="E4" s="14">
         <v>999</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="14">
         <v>987654321</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="14">
         <v>900000000</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" t="s" s="9">
-        <v>38</v>
-      </c>
-      <c r="N4" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="O4" s="11"/>
-      <c r="P4" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="11"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" t="s" s="13">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="8">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s" s="12">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s" s="13">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s" s="13">
+        <v>46</v>
+      </c>
+      <c r="E5" s="14">
         <v>0</v>
       </c>
-      <c r="F5" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="F5" s="15"/>
+      <c r="G5" t="s" s="13">
+        <v>47</v>
+      </c>
+      <c r="H5" s="14">
         <v>912345678</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="K5" s="11"/>
-      <c r="L5" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="M5" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" t="s" s="13">
+        <v>48</v>
+      </c>
+      <c r="L5" s="15"/>
+      <c r="M5" t="s" s="13">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s" s="13">
+        <v>50</v>
+      </c>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="23"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="23"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="23"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="" tooltip="" display="kk@example.com"/>
     <hyperlink ref="D4" r:id="rId2" location="" tooltip="" display="kk@example.com"/>
     <hyperlink ref="C5" r:id="rId3" location="" tooltip="" display="zz@example.com"/>
     <hyperlink ref="D5" r:id="rId4" location="" tooltip="" display="zz@example.com"/>
-    <hyperlink ref="F5" r:id="rId5" location="" tooltip="" display="sales@example.com"/>
+    <hyperlink ref="G5" r:id="rId5" location="" tooltip="" display="sales@example.com"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
test: fix test xlsx data & setup/teardown cycle
</commit_message>
<xml_diff>
--- a/test/tasker/importer/test-member-import-data.xlsx
+++ b/test/tasker/importer/test-member-import-data.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
-  <si>
-    <t>test-member-import-data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>流水號</t>
   </si>
@@ -247,12 +244,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -264,28 +261,6 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -302,13 +277,13 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -317,13 +292,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -332,98 +337,38 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -432,7 +377,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -440,30 +385,30 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right/>
       <top/>
@@ -480,7 +425,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top/>
       <bottom/>
@@ -488,10 +433,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top/>
       <bottom/>
@@ -499,12 +444,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,31 +458,31 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,89 +492,74 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -649,12 +579,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1719,7 +1649,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1741,342 +1671,316 @@
     <col min="20" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="6"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s" s="2">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="7">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="Q2" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="R2" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="S2" t="s" s="7">
+      <c r="A2" t="s" s="3">
         <v>19</v>
       </c>
+      <c r="B2" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="Q2" t="s" s="5">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s" s="5">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="P3" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="Q3" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="R3" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="S3" t="s" s="10">
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s" s="7">
         <v>38</v>
       </c>
+      <c r="C3" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="E3" s="9">
+        <v>999</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9">
+        <v>987654321</v>
+      </c>
+      <c r="I3" s="9">
+        <v>900000000</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" t="s" s="8">
+        <v>40</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3" t="s" s="8">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s" s="8">
+        <v>42</v>
+      </c>
+      <c r="P3" s="10"/>
+      <c r="Q3" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" t="s" s="12">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s" s="13">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s" s="13">
-        <v>40</v>
-      </c>
-      <c r="E4" s="14">
-        <v>999</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="14">
-        <v>987654321</v>
-      </c>
-      <c r="I4" s="14">
-        <v>900000000</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" t="s" s="13">
-        <v>41</v>
-      </c>
-      <c r="M4" s="15"/>
-      <c r="N4" t="s" s="13">
-        <v>42</v>
-      </c>
-      <c r="O4" t="s" s="13">
-        <v>43</v>
-      </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" t="s" s="13">
+      <c r="A4" s="6"/>
+      <c r="B4" t="s" s="7">
         <v>44</v>
       </c>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
+      <c r="C4" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" t="s" s="8">
+        <v>46</v>
+      </c>
+      <c r="H4" s="9">
+        <v>912345678</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" t="s" s="8">
+        <v>48</v>
+      </c>
+      <c r="N4" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
+    <row r="5" ht="14.7" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" t="s" s="12">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s" s="13">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s" s="13">
-        <v>46</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" t="s" s="13">
-        <v>47</v>
-      </c>
-      <c r="H5" s="14">
-        <v>912345678</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" t="s" s="13">
-        <v>48</v>
-      </c>
-      <c r="L5" s="15"/>
-      <c r="M5" t="s" s="13">
-        <v>49</v>
-      </c>
-      <c r="N5" t="s" s="13">
-        <v>50</v>
-      </c>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="14"/>
     </row>
     <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="19"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="18"/>
     </row>
     <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="23"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="18"/>
     </row>
     <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="23"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="18"/>
     </row>
     <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="23"/>
-    </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="27"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" location="" tooltip="" display="kk@example.com"/>
-    <hyperlink ref="D4" r:id="rId2" location="" tooltip="" display="kk@example.com"/>
-    <hyperlink ref="C5" r:id="rId3" location="" tooltip="" display="zz@example.com"/>
-    <hyperlink ref="D5" r:id="rId4" location="" tooltip="" display="zz@example.com"/>
-    <hyperlink ref="G5" r:id="rId5" location="" tooltip="" display="sales@example.com"/>
+    <hyperlink ref="C3" r:id="rId1" location="" tooltip="" display="kk@example.com"/>
+    <hyperlink ref="D3" r:id="rId2" location="" tooltip="" display="kk@example.com"/>
+    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="zz@example.com"/>
+    <hyperlink ref="D4" r:id="rId4" location="" tooltip="" display="zz@example.com"/>
+    <hyperlink ref="G4" r:id="rId5" location="" tooltip="" display="sales@example.com"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
test: e2e case for encoding issue
</commit_message>
<xml_diff>
--- a/test/tasker/importer/test-member-import-data.xlsx
+++ b/test/tasker/importer/test-member-import-data.xlsx
@@ -144,7 +144,7 @@
     <t>工程</t>
   </si>
   <si>
-    <t>test-category</t>
+    <t>測試分類</t>
   </si>
   <si>
     <t>前端工程</t>
@@ -249,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -486,13 +486,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -561,6 +598,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1649,7 +1695,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1974,6 +2020,27 @@
       <c r="R9" s="21"/>
       <c r="S9" s="22"/>
     </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="25"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" location="" tooltip="" display="kk@example.com"/>

</xml_diff>